<commit_message>
simple version of fc tier 2
</commit_message>
<xml_diff>
--- a/inputs/data_raw/Data_SJFC_Decrements_AV2020.xlsx
+++ b/inputs/data_raw/Data_SJFC_Decrements_AV2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Proj_CAPlans\model_SJ\inputs\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF6A17C-F0B6-4990-99E5-4440E398000B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA49FDE-C477-43DA-A549-7F7857F182B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1845" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1845" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ratios" sheetId="43" r:id="rId1"/>
@@ -1008,16 +1008,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>448349</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>162267</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>257849</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>124167</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1040,7 +1040,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6915150" y="1714500"/>
+          <a:off x="5505450" y="1104900"/>
           <a:ext cx="4829849" cy="2448267"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1106,16 +1106,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>819150</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>1057960</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>162392</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>315010</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>29042</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1138,7 +1138,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4714875" y="4829175"/>
+          <a:off x="9382125" y="2200275"/>
           <a:ext cx="4906060" cy="3343742"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1926,7 +1926,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F0179D-30E8-4C62-9A5E-014F54719930}">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C8" sqref="C8:H24"/>
     </sheetView>
   </sheetViews>
@@ -2857,7 +2857,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10:F17"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2963,7 +2963,7 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D20"/>
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3508,7 +3508,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3701,7 +3701,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V15" sqref="V15"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4128,7 +4128,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4579,10 +4579,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3AE2EB2-CA42-4FE6-8F24-6446CEAEA505}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4590,12 +4590,12 @@
     <col min="1" max="1" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -4603,7 +4603,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -4611,7 +4611,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -4619,7 +4619,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>5</v>
       </c>
@@ -4627,67 +4627,99 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>25</v>
       </c>
       <c r="E7">
+        <f>G7/100</f>
+        <v>2.72E-4</v>
+      </c>
+      <c r="G7">
         <v>2.7199999999999998E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>30</v>
       </c>
       <c r="E8">
+        <f t="shared" ref="E8:E14" si="0">G8/100</f>
+        <v>3.0299999999999999E-4</v>
+      </c>
+      <c r="G8">
         <v>3.0300000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>35</v>
       </c>
       <c r="E9">
+        <f t="shared" si="0"/>
+        <v>6.1300000000000005E-4</v>
+      </c>
+      <c r="G9">
         <v>6.13E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D10">
         <v>40</v>
       </c>
       <c r="E10">
+        <f t="shared" si="0"/>
+        <v>1.366E-3</v>
+      </c>
+      <c r="G10">
         <v>0.1366</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>45</v>
       </c>
       <c r="E11">
+        <f t="shared" si="0"/>
+        <v>2.519E-3</v>
+      </c>
+      <c r="G11">
         <v>0.25190000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D12">
         <v>50</v>
       </c>
       <c r="E12">
+        <f t="shared" si="0"/>
+        <v>3.2400000000000003E-3</v>
+      </c>
+      <c r="G12">
         <v>0.32400000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D13">
         <v>55</v>
       </c>
       <c r="E13">
+        <f t="shared" si="0"/>
+        <v>2.6310000000000001E-3</v>
+      </c>
+      <c r="G13">
         <v>0.2631</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D14">
         <v>60</v>
       </c>
       <c r="E14">
+        <f t="shared" si="0"/>
+        <v>2.1909999999999998E-3</v>
+      </c>
+      <c r="G14">
         <v>0.21909999999999999</v>
       </c>
     </row>
@@ -4704,8 +4736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{140C462A-14EE-4CAF-AB62-253A6557DD8D}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4889,7 +4921,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4940,7 +4972,7 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>